<commit_message>
bug 33176 : reading date and number fields
git-svn-id: http://code.jaspersoft.com/svn/repos/jasperreports/trunk/jasperreports@6311 76e25fc1-081a-0410-bb1b-c96bc70638b7
</commit_message>
<xml_diff>
--- a/demo/samples/xlsxdatasource/data/MultisheetXlsxDataSource.data.xlsx
+++ b/demo/samples/xlsxdatasource/data/MultisheetXlsxDataSource.data.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15480" windowHeight="11640" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="XlsxDataSource1" sheetId="1" r:id="rId1"/>
     <sheet name="XlsxDataSource2" sheetId="2" r:id="rId2"/>
     <sheet name="XlsxDataSource3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -241,325 +241,27 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -567,207 +269,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1063,23 +577,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125"/>
+    <col min="2" max="2" width="10.85546875"/>
+    <col min="3" max="3" width="20.140625"/>
+    <col min="4" max="4" width="23.85546875"/>
+    <col min="5" max="5" width="38.28515625"/>
+    <col min="6" max="6" width="28.28515625"/>
+    <col min="7" max="7" width="12.85546875"/>
+    <col min="8" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1095,8 +609,11 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1">
+        <v>40673</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1112,8 +629,11 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <v>41375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1129,8 +649,11 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>40980</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1146,8 +669,11 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>41407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1163,8 +689,11 @@
       <c r="F5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>40708</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1180,8 +709,11 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>41470</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1197,8 +729,11 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>41137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1214,8 +749,11 @@
       <c r="F8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>41564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1231,8 +769,11 @@
       <c r="F9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>40865</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1248,30 +789,36 @@
       <c r="F10" t="s">
         <v>7</v>
       </c>
+      <c r="G10" s="1">
+        <v>41627</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD65525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125"/>
+    <col min="3" max="3" width="19.42578125"/>
+    <col min="4" max="4" width="27"/>
+    <col min="5" max="5" width="22.140625"/>
+    <col min="6" max="6" width="16"/>
+    <col min="7" max="7" width="11.140625"/>
+    <col min="8" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1287,8 +834,11 @@
       <c r="F1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1">
+        <v>40673</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1304,8 +854,11 @@
       <c r="F2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <v>41375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1321,8 +874,11 @@
       <c r="F3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>40980</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1338,8 +894,11 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>41407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1355,8 +914,11 @@
       <c r="F5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>40708</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1372,8 +934,11 @@
       <c r="F6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>41470</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1389,8 +954,11 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>41137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1406,8 +974,11 @@
       <c r="F8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>41564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1423,30 +994,37 @@
       <c r="F9" t="s">
         <v>7</v>
       </c>
+      <c r="G9" s="1">
+        <v>40865</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625"/>
+    <col min="2" max="2" width="8.5703125"/>
+    <col min="3" max="3" width="14.140625"/>
+    <col min="4" max="4" width="20.85546875"/>
+    <col min="5" max="5" width="23.28515625"/>
+    <col min="6" max="6" width="21.140625"/>
+    <col min="7" max="7" width="12.7109375"/>
+    <col min="8" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1462,8 +1040,11 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1">
+        <v>40673</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1479,8 +1060,11 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <v>41375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1496,8 +1080,11 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>40980</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1513,8 +1100,11 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>41407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1530,8 +1120,11 @@
       <c r="F5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>40708</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1547,8 +1140,11 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>41470</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1564,8 +1160,11 @@
       <c r="F7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>41137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1581,8 +1180,11 @@
       <c r="F8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>41564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1598,8 +1200,11 @@
       <c r="F9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>40865</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1615,8 +1220,11 @@
       <c r="F10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <v>41627</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1632,8 +1240,12 @@
       <c r="F11" t="s">
         <v>3</v>
       </c>
+      <c r="G11" s="1">
+        <v>41049</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>